<commit_message>
add pH to substrate characterization of DBFZ measurements
</commit_message>
<xml_diff>
--- a/data/data_in/substrate_characterization_dbfz.xlsx
+++ b/data/data_in/substrate_characterization_dbfz.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shellmann\Desktop\Substrat-Daten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shellmann\SimonsHardDriveSpeicher\GIT\ad_meal_prep_control\data\data_in\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23ACE31A-BC3D-4E22-8435-CE12111FAC13}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68508E4-7FB3-416D-87A2-978D9C0F3B1F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{AEE4862D-4A3E-49D3-987F-015B00AA3EF1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" firstSheet="3" activeTab="4" xr2:uid="{AEE4862D-4A3E-49D3-987F-015B00AA3EF1}"/>
   </bookViews>
   <sheets>
     <sheet name="maize_silage" sheetId="1" r:id="rId1"/>
@@ -1085,7 +1085,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1093,19 +1093,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1" xr:uid="{FD6B50C5-6791-445E-AFB3-554B37CB7B71}"/>
   </cellStyles>
   <dxfs count="3">
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color indexed="9"/>
-      </font>
-    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1119,6 +1114,13 @@
           <bgColor theme="0" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color indexed="9"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1432,9 +1434,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A464897B-AA9E-468D-815C-0C802AF1F274}">
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C2" sqref="C2:J11"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="K1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1618,6 +1620,9 @@
       <c r="J3" s="2">
         <v>12.412630568403891</v>
       </c>
+      <c r="K3" s="2">
+        <v>4.0599999999999996</v>
+      </c>
       <c r="L3" t="s">
         <v>73</v>
       </c>
@@ -1783,6 +1788,9 @@
       <c r="J6" s="2">
         <v>11.165756825070385</v>
       </c>
+      <c r="K6" s="2">
+        <v>3.71</v>
+      </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2"/>
       <c r="P6" s="2"/>
@@ -1825,6 +1833,9 @@
       <c r="J7" s="2">
         <v>11.103242589664891</v>
       </c>
+      <c r="K7" s="2">
+        <v>3.74</v>
+      </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2"/>
       <c r="P7" s="2"/>
@@ -1864,6 +1875,7 @@
       <c r="J8" s="2">
         <v>12.499045494830558</v>
       </c>
+      <c r="K8" s="2"/>
       <c r="N8" s="2"/>
       <c r="O8" s="2"/>
       <c r="P8" s="2"/>
@@ -1948,6 +1960,9 @@
       <c r="J10" s="2">
         <v>12.844774931512783</v>
       </c>
+      <c r="K10" s="2">
+        <v>3.91</v>
+      </c>
       <c r="L10" t="s">
         <v>78</v>
       </c>
@@ -2007,6 +2022,9 @@
       </c>
       <c r="J11" s="2">
         <v>11.72281850304549</v>
+      </c>
+      <c r="K11" s="2">
+        <v>3.99</v>
       </c>
       <c r="L11" t="s">
         <v>79</v>
@@ -2055,7 +2073,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
+      <selection pane="bottomRight" activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2784,6 +2802,9 @@
       <c r="J16" s="6">
         <v>17.064850999618582</v>
       </c>
+      <c r="K16" s="7">
+        <v>4.16</v>
+      </c>
       <c r="L16" t="s">
         <v>30</v>
       </c>
@@ -2870,10 +2891,10 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomRight" activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3461,7 +3482,9 @@
       <c r="J11" s="2">
         <v>15.290544202240401</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="8">
+        <v>3.72</v>
+      </c>
       <c r="L11" t="s">
         <v>83</v>
       </c>
@@ -3522,7 +3545,9 @@
       <c r="J12" s="2">
         <v>15.428540308356219</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="8">
+        <v>3.74</v>
+      </c>
       <c r="L12" t="s">
         <v>84</v>
       </c>
@@ -3583,7 +3608,9 @@
       <c r="J13" s="2">
         <v>15.157152423312887</v>
       </c>
-      <c r="K13" s="2"/>
+      <c r="K13" s="8">
+        <v>3.63</v>
+      </c>
       <c r="L13" t="s">
         <v>85</v>
       </c>
@@ -3644,7 +3671,9 @@
       <c r="J14" s="2">
         <v>17.054760815841739</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="8">
+        <v>3.78</v>
+      </c>
       <c r="U14" t="s">
         <v>80</v>
       </c>
@@ -3680,7 +3709,9 @@
       <c r="J15" s="2">
         <v>15.988067907389333</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="8">
+        <v>3.75</v>
+      </c>
       <c r="U15" t="s">
         <v>80</v>
       </c>
@@ -3716,7 +3747,9 @@
       <c r="J16" s="2">
         <v>16.386240850118366</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="8">
+        <v>3.72</v>
+      </c>
       <c r="U16" t="s">
         <v>80</v>
       </c>
@@ -3725,14 +3758,6 @@
   <sortState ref="A2:U17">
     <sortCondition ref="A2:A17"/>
   </sortState>
-  <conditionalFormatting sqref="K2:K16">
-    <cfRule type="expression" dxfId="2" priority="1">
-      <formula>OR(K2&lt;&gt;0)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>OR(XEB2=1)</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -3744,10 +3769,10 @@
   <dimension ref="A1:U14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomRight" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4521,11 +4546,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C87B9048-F1D1-4E12-A756-955018FCA9B1}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L1" sqref="L1"/>
+      <selection pane="bottomRight" activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="22.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5479,7 +5504,9 @@
         <v>72.714633340062946</v>
       </c>
       <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2">
+        <v>5.76</v>
+      </c>
       <c r="L17" t="s">
         <v>111</v>
       </c>
@@ -5540,7 +5567,9 @@
       <c r="J18" s="2">
         <v>26.862519166235447</v>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2">
+        <v>6.91</v>
+      </c>
       <c r="L18" t="s">
         <v>112</v>
       </c>
@@ -5579,7 +5608,7 @@
     <sortCondition ref="A2:A10"/>
   </sortState>
   <conditionalFormatting sqref="B9">
-    <cfRule type="cellIs" dxfId="0" priority="68" stopIfTrue="1" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="68" stopIfTrue="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>